<commit_message>
Get export date time from filename
</commit_message>
<xml_diff>
--- a/src/test/resources/templatedata.xlsx
+++ b/src/test/resources/templatedata.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emmanuel\Documents\Bodastage\code_repos\pr\boda-ztexlscmparser\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE72ACE-2173-4920-B600-D2339B0B6616}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504" activeTab="3"/>
+    <workbookView xWindow="3084" yWindow="0" windowWidth="19212" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TemplateInfo" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>NE Type:</t>
   </si>
@@ -88,7 +94,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -167,11 +173,19 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -218,7 +232,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,9 +264,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -284,6 +316,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -459,7 +509,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -468,8 +518,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -510,7 +560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -519,8 +569,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -556,11 +606,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -577,25 +627,25 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
+      <c r="A3" s="4">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -648,10 +698,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>